<commit_message>
namemapping beans flatten to row
</commit_message>
<xml_diff>
--- a/W-Domestic Standard Upload Template.xlsx
+++ b/W-Domestic Standard Upload Template.xlsx
@@ -354,7 +354,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="531">
   <si>
     <t>#</t>
   </si>
@@ -1160,132 +1160,6 @@
     <t xml:space="preserve">Shape </t>
   </si>
   <si>
-    <t>cat:0</t>
-  </si>
-  <si>
-    <t>cat:1</t>
-  </si>
-  <si>
-    <t>cat:2</t>
-  </si>
-  <si>
-    <t>cat:3</t>
-  </si>
-  <si>
-    <t>cat:4</t>
-  </si>
-  <si>
-    <t>cat:5</t>
-  </si>
-  <si>
-    <t>cat:6</t>
-  </si>
-  <si>
-    <t>cat:7</t>
-  </si>
-  <si>
-    <t>cat:8</t>
-  </si>
-  <si>
-    <t>cat:9</t>
-  </si>
-  <si>
-    <t>cat:10</t>
-  </si>
-  <si>
-    <t>cat:11</t>
-  </si>
-  <si>
-    <t>cat:12</t>
-  </si>
-  <si>
-    <t>cat:13</t>
-  </si>
-  <si>
-    <t>cat:14</t>
-  </si>
-  <si>
-    <t>cat:15</t>
-  </si>
-  <si>
-    <t>cat:16</t>
-  </si>
-  <si>
-    <t>cat:17</t>
-  </si>
-  <si>
-    <t>cat:18</t>
-  </si>
-  <si>
-    <t>cat:19</t>
-  </si>
-  <si>
-    <t>cat:20</t>
-  </si>
-  <si>
-    <t>cat:21</t>
-  </si>
-  <si>
-    <t>cat:22</t>
-  </si>
-  <si>
-    <t>cat:23</t>
-  </si>
-  <si>
-    <t>cat:24</t>
-  </si>
-  <si>
-    <t>cat:25</t>
-  </si>
-  <si>
-    <t>cat:26</t>
-  </si>
-  <si>
-    <t>cat:27</t>
-  </si>
-  <si>
-    <t>cat:28</t>
-  </si>
-  <si>
-    <t>cat:29</t>
-  </si>
-  <si>
-    <t>cat:30</t>
-  </si>
-  <si>
-    <t>cat:31</t>
-  </si>
-  <si>
-    <t>cat:32</t>
-  </si>
-  <si>
-    <t>cat:33</t>
-  </si>
-  <si>
-    <t>cat:34</t>
-  </si>
-  <si>
-    <t>cat:35</t>
-  </si>
-  <si>
-    <t>cat:36</t>
-  </si>
-  <si>
-    <t>cat:37</t>
-  </si>
-  <si>
-    <t>cat:38</t>
-  </si>
-  <si>
-    <t>cat:39</t>
-  </si>
-  <si>
-    <t>cat:40</t>
-  </si>
-  <si>
-    <t>cat:41</t>
-  </si>
-  <si>
     <t>ven:0</t>
   </si>
   <si>
@@ -1418,13 +1292,565 @@
     <t>ven:43</t>
   </si>
   <si>
-    <t>ven:44</t>
-  </si>
-  <si>
-    <t>ven:45</t>
-  </si>
-  <si>
-    <t>ven:46</t>
+    <t>lab:0</t>
+  </si>
+  <si>
+    <t>lab:1</t>
+  </si>
+  <si>
+    <t>lab:2</t>
+  </si>
+  <si>
+    <t>lab:3</t>
+  </si>
+  <si>
+    <t>lab:4</t>
+  </si>
+  <si>
+    <t>lab:5</t>
+  </si>
+  <si>
+    <t>lab:6</t>
+  </si>
+  <si>
+    <t>lab:7</t>
+  </si>
+  <si>
+    <t>lab:8</t>
+  </si>
+  <si>
+    <t>lab:9</t>
+  </si>
+  <si>
+    <t>lab:10</t>
+  </si>
+  <si>
+    <t>lab:11</t>
+  </si>
+  <si>
+    <t>lab:12</t>
+  </si>
+  <si>
+    <t>lab:13</t>
+  </si>
+  <si>
+    <t>lab:14</t>
+  </si>
+  <si>
+    <t>lab:15</t>
+  </si>
+  <si>
+    <t>lab:16</t>
+  </si>
+  <si>
+    <t>lab:17</t>
+  </si>
+  <si>
+    <t>lab:18</t>
+  </si>
+  <si>
+    <t>lab:19</t>
+  </si>
+  <si>
+    <t>lab:20</t>
+  </si>
+  <si>
+    <t>lab:21</t>
+  </si>
+  <si>
+    <t>lab:22</t>
+  </si>
+  <si>
+    <t>lab:23</t>
+  </si>
+  <si>
+    <t>lab:24</t>
+  </si>
+  <si>
+    <t>lab:25</t>
+  </si>
+  <si>
+    <t>lab:26</t>
+  </si>
+  <si>
+    <t>lab:27</t>
+  </si>
+  <si>
+    <t>lab:28</t>
+  </si>
+  <si>
+    <t>lab:29</t>
+  </si>
+  <si>
+    <t>lab:30</t>
+  </si>
+  <si>
+    <t>lab:31</t>
+  </si>
+  <si>
+    <t>lab:32</t>
+  </si>
+  <si>
+    <t>lab:33</t>
+  </si>
+  <si>
+    <t>lab:34</t>
+  </si>
+  <si>
+    <t>lab:35</t>
+  </si>
+  <si>
+    <t>lab:36</t>
+  </si>
+  <si>
+    <t>lab:37</t>
+  </si>
+  <si>
+    <t>lab:38</t>
+  </si>
+  <si>
+    <t>lab:39</t>
+  </si>
+  <si>
+    <t>lab:40</t>
+  </si>
+  <si>
+    <t>lab:41</t>
+  </si>
+  <si>
+    <t>lab:42</t>
+  </si>
+  <si>
+    <t>lab:43</t>
+  </si>
+  <si>
+    <t>lab:44</t>
+  </si>
+  <si>
+    <t>lab:45</t>
+  </si>
+  <si>
+    <t>lab:46</t>
+  </si>
+  <si>
+    <t>lab:47</t>
+  </si>
+  <si>
+    <t>lab:48</t>
+  </si>
+  <si>
+    <t>lab:49</t>
+  </si>
+  <si>
+    <t>lab:50</t>
+  </si>
+  <si>
+    <t>lab:51</t>
+  </si>
+  <si>
+    <t>lab:52</t>
+  </si>
+  <si>
+    <t>lab:53</t>
+  </si>
+  <si>
+    <t>lab:54</t>
+  </si>
+  <si>
+    <t>lab:55</t>
+  </si>
+  <si>
+    <t>lab:56</t>
+  </si>
+  <si>
+    <t>lab:57</t>
+  </si>
+  <si>
+    <t>lab:58</t>
+  </si>
+  <si>
+    <t>lab:59</t>
+  </si>
+  <si>
+    <t>lab:60</t>
+  </si>
+  <si>
+    <t>lab:61</t>
+  </si>
+  <si>
+    <t>lab:62</t>
+  </si>
+  <si>
+    <t>lab:63</t>
+  </si>
+  <si>
+    <t>lab:64</t>
+  </si>
+  <si>
+    <t>lab:65</t>
+  </si>
+  <si>
+    <t>lab:66</t>
+  </si>
+  <si>
+    <t>lab:67</t>
+  </si>
+  <si>
+    <t>lab:68</t>
+  </si>
+  <si>
+    <t>lab:69</t>
+  </si>
+  <si>
+    <t>lab:70</t>
+  </si>
+  <si>
+    <t>lab:71</t>
+  </si>
+  <si>
+    <t>lab:72</t>
+  </si>
+  <si>
+    <t>lab:73</t>
+  </si>
+  <si>
+    <t>lab:74</t>
+  </si>
+  <si>
+    <t>lab:75</t>
+  </si>
+  <si>
+    <t>lab:76</t>
+  </si>
+  <si>
+    <t>lab:77</t>
+  </si>
+  <si>
+    <t>lab:78</t>
+  </si>
+  <si>
+    <t>lab:79</t>
+  </si>
+  <si>
+    <t>lab:80</t>
+  </si>
+  <si>
+    <t>lab:81</t>
+  </si>
+  <si>
+    <t>lab:82</t>
+  </si>
+  <si>
+    <t>lab:83</t>
+  </si>
+  <si>
+    <t>lab:84</t>
+  </si>
+  <si>
+    <t>lab:85</t>
+  </si>
+  <si>
+    <t>lab:86</t>
+  </si>
+  <si>
+    <t>lab:87</t>
+  </si>
+  <si>
+    <t>lab:88</t>
+  </si>
+  <si>
+    <t>lab:89</t>
+  </si>
+  <si>
+    <t>lab:90</t>
+  </si>
+  <si>
+    <t>lab:91</t>
+  </si>
+  <si>
+    <t>lab:92</t>
+  </si>
+  <si>
+    <t>lab:93</t>
+  </si>
+  <si>
+    <t>lab:94</t>
+  </si>
+  <si>
+    <t>lab:95</t>
+  </si>
+  <si>
+    <t>lab:96</t>
+  </si>
+  <si>
+    <t>lab:97</t>
+  </si>
+  <si>
+    <t>pon:0</t>
+  </si>
+  <si>
+    <t>pon:1</t>
+  </si>
+  <si>
+    <t>pon:2</t>
+  </si>
+  <si>
+    <t>pon:3</t>
+  </si>
+  <si>
+    <t>pon:4</t>
+  </si>
+  <si>
+    <t>pon:5</t>
+  </si>
+  <si>
+    <t>pon:6</t>
+  </si>
+  <si>
+    <t>pon:7</t>
+  </si>
+  <si>
+    <t>pon:8</t>
+  </si>
+  <si>
+    <t>pon:9</t>
+  </si>
+  <si>
+    <t>pon:10</t>
+  </si>
+  <si>
+    <t>pon:11</t>
+  </si>
+  <si>
+    <t>pon:12</t>
+  </si>
+  <si>
+    <t>pon:13</t>
+  </si>
+  <si>
+    <t>pon:14</t>
+  </si>
+  <si>
+    <t>pon:15</t>
+  </si>
+  <si>
+    <t>pon:16</t>
+  </si>
+  <si>
+    <t>pon:17</t>
+  </si>
+  <si>
+    <t>pon:18</t>
+  </si>
+  <si>
+    <t>pon:19</t>
+  </si>
+  <si>
+    <t>pon:20</t>
+  </si>
+  <si>
+    <t>pon:21</t>
+  </si>
+  <si>
+    <t>pon:22</t>
+  </si>
+  <si>
+    <t>pon:23</t>
+  </si>
+  <si>
+    <t>pon:24</t>
+  </si>
+  <si>
+    <t>pon:25</t>
+  </si>
+  <si>
+    <t>pon:26</t>
+  </si>
+  <si>
+    <t>pon:27</t>
+  </si>
+  <si>
+    <t>pon:28</t>
+  </si>
+  <si>
+    <t>pon:29</t>
+  </si>
+  <si>
+    <t>pon:30</t>
+  </si>
+  <si>
+    <t>pon:31</t>
+  </si>
+  <si>
+    <t>pon:32</t>
+  </si>
+  <si>
+    <t>pon:33</t>
+  </si>
+  <si>
+    <t>pon:34</t>
+  </si>
+  <si>
+    <t>pon:35</t>
+  </si>
+  <si>
+    <t>pon:36</t>
+  </si>
+  <si>
+    <t>pon:37</t>
+  </si>
+  <si>
+    <t>pon:38</t>
+  </si>
+  <si>
+    <t>pon:39</t>
+  </si>
+  <si>
+    <t>pon:40</t>
+  </si>
+  <si>
+    <t>pon:41</t>
+  </si>
+  <si>
+    <t>pon:42</t>
+  </si>
+  <si>
+    <t>pon:43</t>
+  </si>
+  <si>
+    <t>pon:44</t>
+  </si>
+  <si>
+    <t>pon:45</t>
+  </si>
+  <si>
+    <t>pon:46</t>
+  </si>
+  <si>
+    <t>pon:47</t>
+  </si>
+  <si>
+    <t>pon:48</t>
+  </si>
+  <si>
+    <t>pon:49</t>
+  </si>
+  <si>
+    <t>pon:50</t>
+  </si>
+  <si>
+    <t>pon:51</t>
+  </si>
+  <si>
+    <t>pon:52</t>
+  </si>
+  <si>
+    <t>pon:53</t>
+  </si>
+  <si>
+    <t>pon:54</t>
+  </si>
+  <si>
+    <t>pon:55</t>
+  </si>
+  <si>
+    <t>pon:56</t>
+  </si>
+  <si>
+    <t>pon:57</t>
+  </si>
+  <si>
+    <t>pon:58</t>
+  </si>
+  <si>
+    <t>pon:59</t>
+  </si>
+  <si>
+    <t>pon:60</t>
+  </si>
+  <si>
+    <t>pon:61</t>
+  </si>
+  <si>
+    <t>pon:62</t>
+  </si>
+  <si>
+    <t>pon:63</t>
+  </si>
+  <si>
+    <t>pon:64</t>
+  </si>
+  <si>
+    <t>pon:65</t>
+  </si>
+  <si>
+    <t>pon:66</t>
+  </si>
+  <si>
+    <t>pon:67</t>
+  </si>
+  <si>
+    <t>pon:68</t>
+  </si>
+  <si>
+    <t>pon:69</t>
+  </si>
+  <si>
+    <t>pon:70</t>
+  </si>
+  <si>
+    <t>pon:71</t>
+  </si>
+  <si>
+    <t>pon:72</t>
+  </si>
+  <si>
+    <t>pon:73</t>
+  </si>
+  <si>
+    <t>pon:74</t>
+  </si>
+  <si>
+    <t>pon:75</t>
+  </si>
+  <si>
+    <t>pon:76</t>
+  </si>
+  <si>
+    <t>pon:77</t>
+  </si>
+  <si>
+    <t>pon:78</t>
+  </si>
+  <si>
+    <t>pon:79</t>
+  </si>
+  <si>
+    <t>pon:80</t>
+  </si>
+  <si>
+    <t>pon:81</t>
+  </si>
+  <si>
+    <t>pon:82</t>
+  </si>
+  <si>
+    <t>pon:83</t>
+  </si>
+  <si>
+    <t>pon:84</t>
+  </si>
+  <si>
+    <t>pon:85</t>
+  </si>
+  <si>
+    <t>pon:86</t>
+  </si>
+  <si>
+    <t>pon:87</t>
+  </si>
+  <si>
+    <t>pon:88</t>
   </si>
   <si>
     <t>red</t>
@@ -6067,7 +6493,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A17F3EB-F212-417F-BA00-A3FB97B2BF77}">
-  <dimension ref="A1:CV88"/>
+  <dimension ref="A1:CV103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
@@ -7373,7 +7799,7 @@
       <c r="AA5" s="43"/>
       <c r="AB5" s="43"/>
       <c r="AC5" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>99.38821754547749</v>
       </c>
       <c r="AD5" s="43"/>
       <c r="AE5" s="43"/>
@@ -7449,1779 +7875,2094 @@
     </row>
     <row r="6">
       <c r="B6" t="n" s="34">
-        <v>44964.71703053241</v>
+        <v>98.52292277781774</v>
       </c>
       <c r="C6" t="s" s="84">
-        <v>292</v>
-      </c>
-      <c r="D6" t="n" s="75">
-        <v>93.95022407623532</v>
+        <v>250</v>
+      </c>
+      <c r="D6" t="s" s="75">
+        <v>294</v>
       </c>
       <c r="E6" t="n" s="76">
-        <v>81.10473061504089</v>
+        <v>30.34952270748129</v>
       </c>
       <c r="F6" t="n" s="76">
-        <v>33.02313233022803</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G6" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H6" t="n" s="78">
-        <v>98.3192035733342</v>
+        <v>31.359052698722202</v>
+      </c>
+      <c r="H6" t="s" s="78">
+        <v>392</v>
       </c>
       <c r="I6" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J6" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K6" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L6" t="s" s="36">
-        <v>250</v>
+        <v>49.583684046730056</v>
+      </c>
+      <c r="L6" t="n" s="36">
+        <v>47.20510775277603</v>
       </c>
       <c r="M6" t="n" s="36">
-        <v>57.085248607474384</v>
+        <v>38.99640828030358</v>
       </c>
       <c r="AC6" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>36.26618920447227</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="n" s="34">
-        <v>44964.71703053241</v>
+        <v>25.841479092038565</v>
       </c>
       <c r="C7" t="s" s="84">
-        <v>293</v>
-      </c>
-      <c r="D7" t="n" s="75">
-        <v>74.59813937180614</v>
+        <v>251</v>
+      </c>
+      <c r="D7" t="s" s="75">
+        <v>295</v>
       </c>
       <c r="E7" t="n" s="76">
-        <v>34.466316545872836</v>
+        <v>9.613815982851037</v>
       </c>
       <c r="F7" t="n" s="76">
-        <v>45.63350665261565</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G7" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H7" t="n" s="78">
-        <v>86.71216303445067</v>
+        <v>80.22660618553962</v>
+      </c>
+      <c r="H7" t="s" s="78">
+        <v>393</v>
       </c>
       <c r="I7" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J7" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K7" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L7" t="s" s="36">
-        <v>251</v>
+        <v>36.27505553976415</v>
+      </c>
+      <c r="L7" t="n" s="36">
+        <v>21.923765380326355</v>
       </c>
       <c r="M7" t="n" s="36">
-        <v>92.77090605560325</v>
+        <v>90.73593899567362</v>
       </c>
       <c r="AC7" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>58.73373702714265</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="n" s="34">
-        <v>44964.71703053241</v>
+        <v>74.16849160472458</v>
       </c>
       <c r="C8" t="s" s="84">
-        <v>294</v>
-      </c>
-      <c r="D8" t="n" s="75">
-        <v>67.25710257752982</v>
+        <v>252</v>
+      </c>
+      <c r="D8" t="s" s="75">
+        <v>296</v>
       </c>
       <c r="E8" t="n" s="76">
-        <v>80.04120205726942</v>
+        <v>78.19827728710564</v>
       </c>
       <c r="F8" t="n" s="76">
-        <v>88.59290032431298</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G8" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H8" t="n" s="78">
-        <v>10.042187714478413</v>
+        <v>77.4117139933034</v>
+      </c>
+      <c r="H8" t="s" s="78">
+        <v>394</v>
       </c>
       <c r="I8" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J8" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K8" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L8" t="s" s="36">
-        <v>252</v>
+        <v>25.00411039997753</v>
+      </c>
+      <c r="L8" t="n" s="36">
+        <v>74.09643843022836</v>
       </c>
       <c r="M8" t="n" s="36">
-        <v>24.477441749571383</v>
+        <v>1.4330109914957534</v>
       </c>
       <c r="AC8" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>42.34759859954411</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="n" s="34">
-        <v>44964.71703053241</v>
+        <v>67.85179904337268</v>
       </c>
       <c r="C9" t="s" s="84">
-        <v>295</v>
-      </c>
-      <c r="D9" t="n" s="75">
-        <v>19.733444060515925</v>
+        <v>253</v>
+      </c>
+      <c r="D9" t="s" s="75">
+        <v>297</v>
       </c>
       <c r="E9" t="n" s="76">
-        <v>69.08886696048987</v>
+        <v>57.7040413260709</v>
       </c>
       <c r="F9" t="n" s="76">
-        <v>15.201549344462762</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G9" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H9" t="n" s="78">
-        <v>90.34703537384118</v>
+        <v>53.92225544207607</v>
+      </c>
+      <c r="H9" t="s" s="78">
+        <v>395</v>
       </c>
       <c r="I9" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J9" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K9" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L9" t="s" s="36">
-        <v>253</v>
+        <v>97.31945632865006</v>
+      </c>
+      <c r="L9" t="n" s="36">
+        <v>98.81998451954772</v>
       </c>
       <c r="M9" t="n" s="36">
-        <v>33.18780393436851</v>
+        <v>3.939720236328581</v>
       </c>
       <c r="AC9" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>41.79133315543272</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="n" s="34">
-        <v>44964.71703053241</v>
+        <v>47.731858342633025</v>
       </c>
       <c r="C10" t="s" s="84">
-        <v>296</v>
-      </c>
-      <c r="D10" t="n" s="75">
-        <v>57.16028601541653</v>
+        <v>254</v>
+      </c>
+      <c r="D10" t="s" s="75">
+        <v>298</v>
       </c>
       <c r="E10" t="n" s="76">
-        <v>1.5867056380474809</v>
+        <v>28.75442646926786</v>
       </c>
       <c r="F10" t="n" s="76">
-        <v>44.79343815871842</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G10" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H10" t="n" s="78">
-        <v>70.6110158279913</v>
+        <v>29.16425887782321</v>
+      </c>
+      <c r="H10" t="s" s="78">
+        <v>396</v>
       </c>
       <c r="I10" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J10" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K10" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L10" t="s" s="36">
-        <v>254</v>
+        <v>8.341918162587426</v>
+      </c>
+      <c r="L10" t="n" s="36">
+        <v>98.48479922256216</v>
       </c>
       <c r="M10" t="n" s="36">
-        <v>18.93155280086809</v>
+        <v>37.262499190282675</v>
       </c>
       <c r="AC10" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>59.117803219132036</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="n" s="34">
-        <v>44964.71703053241</v>
+        <v>77.30567042828375</v>
       </c>
       <c r="C11" t="s" s="84">
-        <v>297</v>
-      </c>
-      <c r="D11" t="n" s="75">
-        <v>17.13481447244324</v>
+        <v>255</v>
+      </c>
+      <c r="D11" t="s" s="75">
+        <v>299</v>
       </c>
       <c r="E11" t="n" s="76">
-        <v>80.02746209570402</v>
+        <v>25.13505043559272</v>
       </c>
       <c r="F11" t="n" s="76">
-        <v>62.611905226883266</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G11" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H11" t="n" s="78">
-        <v>46.21600596959533</v>
+        <v>62.53146692022361</v>
+      </c>
+      <c r="H11" t="s" s="78">
+        <v>397</v>
       </c>
       <c r="I11" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J11" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K11" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L11" t="s" s="36">
-        <v>255</v>
+        <v>18.481330579845423</v>
+      </c>
+      <c r="L11" t="n" s="36">
+        <v>36.452360339172515</v>
       </c>
       <c r="M11" t="n" s="36">
-        <v>23.687897327114193</v>
+        <v>46.298185079089016</v>
       </c>
       <c r="AC11" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>6.367463199821599</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="n" s="34">
-        <v>44964.71703053241</v>
+        <v>71.13708524039319</v>
       </c>
       <c r="C12" t="s" s="84">
-        <v>298</v>
-      </c>
-      <c r="D12" t="n" s="75">
-        <v>25.188044160680157</v>
+        <v>256</v>
+      </c>
+      <c r="D12" t="s" s="75">
+        <v>300</v>
       </c>
       <c r="E12" t="n" s="76">
-        <v>34.009346505892864</v>
+        <v>55.20400241300085</v>
       </c>
       <c r="F12" t="n" s="76">
-        <v>29.476573911060843</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G12" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H12" t="n" s="78">
-        <v>65.73300142560069</v>
+        <v>98.84224703698649</v>
+      </c>
+      <c r="H12" t="s" s="78">
+        <v>398</v>
       </c>
       <c r="I12" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J12" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K12" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L12" t="s" s="36">
-        <v>256</v>
+        <v>3.779599592453542</v>
+      </c>
+      <c r="L12" t="n" s="36">
+        <v>14.234660685231038</v>
       </c>
       <c r="M12" t="n" s="36">
-        <v>42.664314287295035</v>
+        <v>79.38486644665062</v>
       </c>
       <c r="AC12" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>37.60790608431851</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="n" s="34">
-        <v>44964.71703053241</v>
+        <v>56.101550413418444</v>
       </c>
       <c r="C13" t="s" s="84">
-        <v>299</v>
-      </c>
-      <c r="D13" t="n" s="75">
-        <v>65.42473222047211</v>
+        <v>257</v>
+      </c>
+      <c r="D13" t="s" s="75">
+        <v>301</v>
       </c>
       <c r="E13" t="n" s="76">
-        <v>28.223776887919904</v>
+        <v>12.642951927722802</v>
       </c>
       <c r="F13" t="n" s="76">
-        <v>24.884986013857848</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G13" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H13" t="n" s="78">
-        <v>52.10762847322934</v>
+        <v>55.252120947710424</v>
+      </c>
+      <c r="H13" t="s" s="78">
+        <v>399</v>
       </c>
       <c r="I13" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J13" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K13" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L13" t="s" s="36">
-        <v>257</v>
-      </c>
-      <c r="M13" t="n" s="36">
-        <v>59.813930605722156</v>
+        <v>15.168611588762182</v>
+      </c>
+      <c r="L13" t="n" s="36">
+        <v>97.33086715418904</v>
       </c>
       <c r="AC13" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>49.398873790524945</v>
       </c>
     </row>
     <row r="14">
+      <c r="B14" t="n" s="34">
+        <v>66.69649447011837</v>
+      </c>
       <c r="C14" t="s" s="84">
-        <v>300</v>
-      </c>
-      <c r="D14" t="n" s="75">
-        <v>13.385968922892689</v>
+        <v>258</v>
+      </c>
+      <c r="D14" t="s" s="75">
+        <v>302</v>
       </c>
       <c r="E14" t="n" s="76">
-        <v>89.24040252662448</v>
+        <v>88.7488915673344</v>
       </c>
       <c r="F14" t="n" s="76">
-        <v>26.599027002604757</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G14" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H14" t="n" s="78">
-        <v>76.26266286635708</v>
+        <v>50.67508581262303</v>
+      </c>
+      <c r="H14" t="s" s="78">
+        <v>400</v>
       </c>
       <c r="I14" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J14" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K14" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L14" t="s" s="36">
-        <v>258</v>
-      </c>
-      <c r="M14" t="n" s="36">
-        <v>98.10910516779455</v>
+        <v>11.60409057032844</v>
+      </c>
+      <c r="L14" t="n" s="36">
+        <v>84.61614896888857</v>
       </c>
       <c r="AC14" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>82.86075096166591</v>
       </c>
     </row>
     <row r="15">
+      <c r="B15" t="n" s="34">
+        <v>73.78286790253156</v>
+      </c>
       <c r="C15" t="s" s="84">
-        <v>301</v>
-      </c>
-      <c r="D15" t="n" s="75">
-        <v>10.081347708759193</v>
+        <v>259</v>
+      </c>
+      <c r="D15" t="s" s="75">
+        <v>303</v>
       </c>
       <c r="E15" t="n" s="76">
-        <v>44.06044433842311</v>
+        <v>1.2075102557199013</v>
       </c>
       <c r="F15" t="n" s="76">
-        <v>57.84849309871972</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G15" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H15" t="n" s="78">
-        <v>58.49266740498897</v>
+        <v>36.90753298878473</v>
+      </c>
+      <c r="H15" t="s" s="78">
+        <v>401</v>
       </c>
       <c r="I15" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J15" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K15" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L15" t="s" s="36">
-        <v>259</v>
-      </c>
-      <c r="M15" t="n" s="36">
-        <v>13.241269550257185</v>
+        <v>3.573642218823714</v>
+      </c>
+      <c r="L15" t="n" s="36">
+        <v>81.5377220866923</v>
       </c>
       <c r="AC15" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>93.33087984659136</v>
       </c>
     </row>
     <row r="16">
+      <c r="B16" t="n" s="34">
+        <v>83.73784899127087</v>
+      </c>
       <c r="C16" t="s" s="84">
-        <v>302</v>
-      </c>
-      <c r="D16" t="n" s="75">
-        <v>88.97846298298155</v>
+        <v>260</v>
+      </c>
+      <c r="D16" t="s" s="75">
+        <v>304</v>
+      </c>
+      <c r="E16" t="n" s="76">
+        <v>44.23552052269589</v>
       </c>
       <c r="F16" t="n" s="76">
-        <v>57.085976460094166</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G16" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H16" t="n" s="78">
-        <v>40.66460921881827</v>
+        <v>98.12990937626664</v>
+      </c>
+      <c r="H16" t="s" s="78">
+        <v>402</v>
       </c>
       <c r="I16" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J16" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K16" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L16" t="s" s="36">
-        <v>260</v>
-      </c>
-      <c r="M16" t="n" s="36">
-        <v>95.40976236551366</v>
+        <v>74.44714286792272</v>
+      </c>
+      <c r="L16" t="n" s="36">
+        <v>6.3684752303799</v>
       </c>
       <c r="AC16" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>16.731743474138494</v>
       </c>
     </row>
     <row r="17">
+      <c r="B17" t="n" s="34">
+        <v>71.76740189440076</v>
+      </c>
       <c r="C17" t="s" s="84">
-        <v>303</v>
-      </c>
-      <c r="D17" t="n" s="75">
-        <v>98.16701903053897</v>
+        <v>261</v>
+      </c>
+      <c r="D17" t="s" s="75">
+        <v>305</v>
+      </c>
+      <c r="E17" t="n" s="76">
+        <v>31.23123932401096</v>
       </c>
       <c r="F17" t="n" s="76">
-        <v>16.222069347155955</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G17" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H17" t="n" s="78">
-        <v>38.962535598192346</v>
+        <v>7.76117260875937</v>
+      </c>
+      <c r="H17" t="s" s="78">
+        <v>403</v>
       </c>
       <c r="I17" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J17" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K17" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L17" t="s" s="36">
-        <v>261</v>
-      </c>
-      <c r="M17" t="n" s="36">
-        <v>98.67521748687082</v>
+        <v>41.252118302579134</v>
+      </c>
+      <c r="L17" t="n" s="36">
+        <v>90.77275369940618</v>
       </c>
       <c r="AC17" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>38.39328825774319</v>
       </c>
     </row>
     <row r="18">
+      <c r="B18" t="n" s="34">
+        <v>11.113747224337867</v>
+      </c>
       <c r="C18" t="s" s="84">
-        <v>304</v>
+        <v>262</v>
+      </c>
+      <c r="D18" t="s" s="75">
+        <v>306</v>
+      </c>
+      <c r="E18" t="n" s="76">
+        <v>97.1088776258087</v>
       </c>
       <c r="F18" t="n" s="76">
-        <v>69.10632382163436</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G18" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H18" t="n" s="78">
-        <v>91.2043988293895</v>
+        <v>20.08847738244739</v>
+      </c>
+      <c r="H18" t="s" s="78">
+        <v>404</v>
       </c>
       <c r="I18" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.93705337963</v>
       </c>
       <c r="J18" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K18" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L18" t="s" s="36">
-        <v>262</v>
-      </c>
-      <c r="M18" t="n" s="36">
-        <v>3.132440174193407</v>
+        <v>66.05848726556482</v>
+      </c>
+      <c r="L18" t="n" s="36">
+        <v>61.51464658614631</v>
       </c>
       <c r="AC18" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>42.22521446990783</v>
       </c>
     </row>
     <row r="19">
+      <c r="B19" t="n" s="34">
+        <v>28.028180032093875</v>
+      </c>
       <c r="C19" t="s" s="84">
-        <v>305</v>
+        <v>263</v>
+      </c>
+      <c r="D19" t="s" s="75">
+        <v>307</v>
+      </c>
+      <c r="E19" t="n" s="76">
+        <v>73.07847021478554</v>
       </c>
       <c r="F19" t="n" s="76">
-        <v>25.305303531633793</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="G19" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H19" t="n" s="78">
-        <v>5.074364790842123</v>
-      </c>
-      <c r="I19" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>20.836676992228544</v>
+      </c>
+      <c r="H19" t="s" s="78">
+        <v>405</v>
       </c>
       <c r="J19" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K19" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L19" t="s" s="36">
-        <v>263</v>
-      </c>
-      <c r="M19" t="n" s="36">
-        <v>1.2369270950963074</v>
+        <v>26.933793593610268</v>
+      </c>
+      <c r="L19" t="n" s="36">
+        <v>58.84699230929799</v>
       </c>
       <c r="AC19" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>66.45567595829098</v>
       </c>
     </row>
     <row r="20">
+      <c r="B20" t="n" s="34">
+        <v>2.357655322458785</v>
+      </c>
       <c r="C20" t="s" s="84">
-        <v>306</v>
-      </c>
-      <c r="F20" t="n" s="76">
-        <v>35.62462160260977</v>
+        <v>264</v>
+      </c>
+      <c r="D20" t="s" s="75">
+        <v>308</v>
+      </c>
+      <c r="E20" t="n" s="76">
+        <v>19.041647969655706</v>
       </c>
       <c r="G20" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H20" t="n" s="78">
-        <v>68.21537973393016</v>
-      </c>
-      <c r="I20" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>38.05942093908739</v>
+      </c>
+      <c r="H20" t="s" s="78">
+        <v>406</v>
       </c>
       <c r="J20" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K20" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L20" t="s" s="36">
-        <v>264</v>
-      </c>
-      <c r="M20" t="n" s="36">
-        <v>60.426564473153356</v>
+        <v>17.12512656870604</v>
+      </c>
+      <c r="L20" t="n" s="36">
+        <v>38.07098605925937</v>
       </c>
       <c r="AC20" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>1.2257701246430885</v>
       </c>
     </row>
     <row r="21">
+      <c r="B21" t="n" s="34">
+        <v>9.4471900079522</v>
+      </c>
       <c r="C21" t="s" s="84">
-        <v>307</v>
-      </c>
-      <c r="F21" t="n" s="76">
-        <v>4.328264542136962</v>
+        <v>265</v>
+      </c>
+      <c r="D21" t="s" s="75">
+        <v>309</v>
+      </c>
+      <c r="E21" t="n" s="76">
+        <v>26.194213638999564</v>
       </c>
       <c r="G21" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H21" t="n" s="78">
-        <v>3.064779481740232</v>
-      </c>
-      <c r="I21" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>82.84835109435481</v>
+      </c>
+      <c r="H21" t="s" s="78">
+        <v>407</v>
       </c>
       <c r="J21" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44964.937053368056</v>
       </c>
       <c r="K21" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L21" t="s" s="36">
-        <v>265</v>
-      </c>
-      <c r="M21" t="n" s="36">
-        <v>0.0442484183008629</v>
+        <v>87.62876320595274</v>
+      </c>
+      <c r="L21" t="n" s="36">
+        <v>46.30194845691216</v>
       </c>
       <c r="AC21" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>51.922622686490314</v>
       </c>
     </row>
     <row r="22">
+      <c r="B22" t="n" s="34">
+        <v>8.309872660193385</v>
+      </c>
       <c r="C22" t="s" s="84">
-        <v>308</v>
-      </c>
-      <c r="F22" t="n" s="76">
-        <v>66.9704702541027</v>
+        <v>266</v>
+      </c>
+      <c r="D22" t="s" s="75">
+        <v>310</v>
+      </c>
+      <c r="E22" t="n" s="76">
+        <v>13.096962504732002</v>
       </c>
       <c r="G22" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H22" t="n" s="78">
-        <v>98.85167701337066</v>
-      </c>
-      <c r="I22" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J22" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>74.6283391327624</v>
+      </c>
+      <c r="H22" t="s" s="78">
+        <v>408</v>
       </c>
       <c r="K22" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L22" t="s" s="36">
-        <v>266</v>
-      </c>
-      <c r="M22" t="n" s="36">
-        <v>58.06610395800737</v>
+        <v>18.15827042516196</v>
+      </c>
+      <c r="L22" t="n" s="36">
+        <v>80.04353929007333</v>
       </c>
       <c r="AC22" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>78.04966861496592</v>
       </c>
     </row>
     <row r="23">
+      <c r="B23" t="n" s="34">
+        <v>65.90689897880512</v>
+      </c>
       <c r="C23" t="s" s="84">
-        <v>309</v>
-      </c>
-      <c r="F23" t="n" s="76">
-        <v>20.716649262904397</v>
+        <v>267</v>
+      </c>
+      <c r="D23" t="s" s="75">
+        <v>311</v>
+      </c>
+      <c r="E23" t="n" s="76">
+        <v>84.66084770323553</v>
       </c>
       <c r="G23" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H23" t="n" s="78">
-        <v>25.521681333903643</v>
-      </c>
-      <c r="I23" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J23" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>88.32418231349449</v>
+      </c>
+      <c r="H23" t="s" s="78">
+        <v>409</v>
       </c>
       <c r="K23" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L23" t="s" s="36">
-        <v>267</v>
-      </c>
-      <c r="M23" t="n" s="36">
-        <v>42.25503809190264</v>
+        <v>60.430048048433925</v>
+      </c>
+      <c r="L23" t="n" s="36">
+        <v>93.89352603904901</v>
       </c>
       <c r="AC23" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>42.36554656071551</v>
       </c>
     </row>
     <row r="24">
+      <c r="B24" t="n" s="34">
+        <v>50.3458147365464</v>
+      </c>
       <c r="C24" t="s" s="84">
-        <v>310</v>
-      </c>
-      <c r="F24" t="n" s="76">
-        <v>95.20831079052127</v>
+        <v>268</v>
+      </c>
+      <c r="D24" t="s" s="75">
+        <v>312</v>
+      </c>
+      <c r="E24" t="n" s="76">
+        <v>90.0831785203403</v>
       </c>
       <c r="G24" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H24" t="n" s="78">
-        <v>73.25886900566303</v>
-      </c>
-      <c r="I24" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J24" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>79.40385205307615</v>
+      </c>
+      <c r="H24" t="s" s="78">
+        <v>410</v>
       </c>
       <c r="K24" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L24" t="s" s="36">
-        <v>268</v>
-      </c>
-      <c r="M24" t="n" s="36">
-        <v>61.32712163237277</v>
+        <v>72.38614137055093</v>
+      </c>
+      <c r="L24" t="n" s="36">
+        <v>96.10396973368594</v>
       </c>
       <c r="AC24" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>85.44573190177822</v>
       </c>
     </row>
     <row r="25">
+      <c r="B25" t="n" s="34">
+        <v>13.928813586938016</v>
+      </c>
       <c r="C25" t="s" s="84">
-        <v>311</v>
-      </c>
-      <c r="F25" t="n" s="76">
-        <v>51.79874451579217</v>
+        <v>269</v>
+      </c>
+      <c r="D25" t="s" s="75">
+        <v>313</v>
+      </c>
+      <c r="E25" t="n" s="76">
+        <v>38.89614674481512</v>
       </c>
       <c r="G25" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H25" t="n" s="78">
-        <v>50.57449142037219</v>
-      </c>
-      <c r="I25" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J25" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>14.888884412301252</v>
+      </c>
+      <c r="H25" t="s" s="78">
+        <v>411</v>
       </c>
       <c r="K25" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L25" t="s" s="36">
-        <v>269</v>
-      </c>
-      <c r="M25" t="n" s="36">
-        <v>45.095233427266415</v>
+        <v>99.26207609798423</v>
+      </c>
+      <c r="L25" t="n" s="36">
+        <v>16.34683696079451</v>
       </c>
       <c r="AC25" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>76.53510926432358</v>
       </c>
     </row>
     <row r="26">
+      <c r="B26" t="n" s="34">
+        <v>95.83973539526501</v>
+      </c>
       <c r="C26" t="s" s="84">
-        <v>312</v>
-      </c>
-      <c r="F26" t="n" s="76">
-        <v>25.39659228214396</v>
+        <v>270</v>
+      </c>
+      <c r="D26" t="s" s="75">
+        <v>314</v>
+      </c>
+      <c r="E26" t="n" s="76">
+        <v>95.94797113619117</v>
       </c>
       <c r="G26" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H26" t="n" s="78">
-        <v>41.859659320856416</v>
-      </c>
-      <c r="I26" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J26" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>5.785440773602701</v>
+      </c>
+      <c r="H26" t="s" s="78">
+        <v>412</v>
       </c>
       <c r="K26" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L26" t="s" s="36">
-        <v>270</v>
-      </c>
-      <c r="M26" t="n" s="36">
-        <v>21.635509452602307</v>
+        <v>63.888519761875806</v>
+      </c>
+      <c r="L26" t="n" s="36">
+        <v>24.563123817759024</v>
       </c>
       <c r="AC26" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>54.17885914556141</v>
       </c>
     </row>
     <row r="27">
+      <c r="B27" t="n" s="34">
+        <v>12.160883078183515</v>
+      </c>
       <c r="C27" t="s" s="84">
-        <v>313</v>
-      </c>
-      <c r="F27" t="n" s="76">
-        <v>16.092862003911623</v>
+        <v>271</v>
+      </c>
+      <c r="D27" t="s" s="75">
+        <v>315</v>
+      </c>
+      <c r="E27" t="n" s="76">
+        <v>6.502814471921303</v>
       </c>
       <c r="G27" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H27" t="n" s="78">
-        <v>11.919964886112</v>
-      </c>
-      <c r="I27" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J27" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>92.94093226204755</v>
+      </c>
+      <c r="H27" t="s" s="78">
+        <v>413</v>
       </c>
       <c r="K27" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L27" t="s" s="36">
-        <v>271</v>
-      </c>
-      <c r="M27" t="n" s="36">
-        <v>54.87751082238016</v>
+        <v>10.314483087844906</v>
+      </c>
+      <c r="L27" t="n" s="36">
+        <v>38.69001585614406</v>
       </c>
       <c r="AC27" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>9.373009947671829</v>
       </c>
     </row>
     <row r="28">
+      <c r="B28" t="n" s="34">
+        <v>20.193349340626987</v>
+      </c>
       <c r="C28" t="s" s="84">
-        <v>314</v>
-      </c>
-      <c r="F28" t="n" s="76">
-        <v>3.0554362463300233</v>
+        <v>272</v>
+      </c>
+      <c r="D28" t="s" s="75">
+        <v>316</v>
+      </c>
+      <c r="E28" t="n" s="76">
+        <v>12.29696516266321</v>
       </c>
       <c r="G28" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H28" t="n" s="78">
-        <v>23.809650189320553</v>
-      </c>
-      <c r="I28" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J28" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>57.08734926583973</v>
+      </c>
+      <c r="H28" t="s" s="78">
+        <v>414</v>
       </c>
       <c r="K28" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L28" t="s" s="36">
-        <v>272</v>
-      </c>
-      <c r="M28" t="n" s="36">
-        <v>27.541729924269585</v>
+        <v>56.42300518530684</v>
+      </c>
+      <c r="L28" t="n" s="36">
+        <v>55.74580984800117</v>
       </c>
       <c r="AC28" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>10.35447120475197</v>
       </c>
     </row>
     <row r="29">
+      <c r="B29" t="n" s="34">
+        <v>16.666589095965122</v>
+      </c>
       <c r="C29" t="s" s="84">
-        <v>315</v>
-      </c>
-      <c r="F29" t="n" s="76">
-        <v>59.57766384918393</v>
+        <v>273</v>
+      </c>
+      <c r="D29" t="s" s="75">
+        <v>317</v>
+      </c>
+      <c r="E29" t="n" s="76">
+        <v>99.36391076882013</v>
       </c>
       <c r="G29" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H29" t="n" s="78">
-        <v>46.546600781132156</v>
-      </c>
-      <c r="I29" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J29" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>93.64029970180223</v>
+      </c>
+      <c r="H29" t="s" s="78">
+        <v>415</v>
       </c>
       <c r="K29" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L29" t="s" s="36">
-        <v>273</v>
-      </c>
-      <c r="M29" t="n" s="36">
-        <v>46.82637253357424</v>
+        <v>40.222615585529574</v>
+      </c>
+      <c r="L29" t="n" s="36">
+        <v>66.30302013847978</v>
       </c>
       <c r="AC29" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>76.0233456122927</v>
       </c>
     </row>
     <row r="30">
+      <c r="B30" t="n" s="34">
+        <v>99.71704109112122</v>
+      </c>
       <c r="C30" t="s" s="84">
-        <v>316</v>
-      </c>
-      <c r="F30" t="n" s="76">
-        <v>45.53872533306029</v>
+        <v>274</v>
+      </c>
+      <c r="D30" t="s" s="75">
+        <v>318</v>
+      </c>
+      <c r="E30" t="n" s="76">
+        <v>86.631753633222</v>
       </c>
       <c r="G30" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H30" t="n" s="78">
-        <v>66.53832911842889</v>
-      </c>
-      <c r="I30" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J30" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>90.09366422789739</v>
+      </c>
+      <c r="H30" t="s" s="78">
+        <v>416</v>
       </c>
       <c r="K30" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L30" t="s" s="36">
-        <v>274</v>
-      </c>
-      <c r="M30" t="n" s="36">
-        <v>14.100825717722376</v>
+        <v>96.62081358168686</v>
+      </c>
+      <c r="L30" t="n" s="36">
+        <v>39.21363026665799</v>
       </c>
       <c r="AC30" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>70.97444516770126</v>
       </c>
     </row>
     <row r="31">
+      <c r="B31" t="n" s="34">
+        <v>92.75066563963655</v>
+      </c>
       <c r="C31" t="s" s="84">
-        <v>317</v>
+        <v>275</v>
+      </c>
+      <c r="D31" t="s" s="75">
+        <v>319</v>
+      </c>
+      <c r="E31" t="n" s="76">
+        <v>2.3193568538293796</v>
       </c>
       <c r="G31" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H31" t="n" s="78">
-        <v>43.922234567783356</v>
-      </c>
-      <c r="I31" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J31" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>5.320329759376097</v>
+      </c>
+      <c r="H31" t="s" s="78">
+        <v>417</v>
       </c>
       <c r="K31" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L31" t="s" s="36">
-        <v>275</v>
-      </c>
-      <c r="M31" t="n" s="36">
-        <v>59.321894098454266</v>
+        <v>18.464384510398414</v>
+      </c>
+      <c r="L31" t="n" s="36">
+        <v>84.32527477711366</v>
       </c>
       <c r="AC31" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>2.072998404698201</v>
       </c>
     </row>
     <row r="32">
+      <c r="B32" t="n" s="34">
+        <v>84.00051194117079</v>
+      </c>
       <c r="C32" t="s" s="84">
-        <v>318</v>
+        <v>276</v>
+      </c>
+      <c r="D32" t="s" s="75">
+        <v>320</v>
+      </c>
+      <c r="E32" t="n" s="76">
+        <v>10.468742793190932</v>
       </c>
       <c r="G32" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H32" t="n" s="78">
-        <v>39.125230268253695</v>
-      </c>
-      <c r="I32" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J32" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>78.24659663121443</v>
+      </c>
+      <c r="H32" t="s" s="78">
+        <v>418</v>
       </c>
       <c r="K32" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L32" t="s" s="36">
-        <v>276</v>
-      </c>
-      <c r="M32" t="n" s="36">
-        <v>57.47255593128011</v>
+        <v>88.1319816710034</v>
+      </c>
+      <c r="L32" t="n" s="36">
+        <v>16.643573038725044</v>
       </c>
       <c r="AC32" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>74.20171909975247</v>
       </c>
     </row>
     <row r="33">
+      <c r="B33" t="n" s="34">
+        <v>50.504767117609596</v>
+      </c>
       <c r="C33" t="s" s="84">
-        <v>319</v>
+        <v>277</v>
+      </c>
+      <c r="D33" t="s" s="75">
+        <v>321</v>
+      </c>
+      <c r="E33" t="n" s="76">
+        <v>13.597248746977353</v>
       </c>
       <c r="G33" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H33" t="n" s="78">
-        <v>75.2957535938529</v>
-      </c>
-      <c r="I33" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="J33" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>16.807833904955118</v>
+      </c>
+      <c r="H33" t="s" s="78">
+        <v>419</v>
       </c>
       <c r="K33" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L33" t="s" s="36">
-        <v>277</v>
-      </c>
-      <c r="M33" t="n" s="36">
-        <v>74.18027434187213</v>
-      </c>
-      <c r="AC33" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>39.25391321752796</v>
+      </c>
+      <c r="L33" t="n" s="36">
+        <v>89.0701297551135</v>
       </c>
     </row>
     <row r="34">
+      <c r="B34" t="n" s="34">
+        <v>41.34111720315781</v>
+      </c>
       <c r="C34" t="s" s="84">
-        <v>320</v>
+        <v>278</v>
+      </c>
+      <c r="D34" t="s" s="75">
+        <v>322</v>
+      </c>
+      <c r="E34" t="n" s="76">
+        <v>8.471325561757093</v>
       </c>
       <c r="G34" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H34" t="n" s="78">
-        <v>14.106089242386233</v>
-      </c>
-      <c r="I34" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>44.69961890563751</v>
+      </c>
+      <c r="H34" t="s" s="78">
+        <v>420</v>
       </c>
       <c r="K34" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L34" t="s" s="36">
-        <v>278</v>
-      </c>
-      <c r="M34" t="n" s="36">
-        <v>66.88713454709769</v>
-      </c>
-      <c r="AC34" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>59.09848679443913</v>
+      </c>
+      <c r="L34" t="n" s="36">
+        <v>87.27158261933978</v>
       </c>
     </row>
     <row r="35">
+      <c r="B35" t="n" s="34">
+        <v>13.46872122020989</v>
+      </c>
       <c r="C35" t="s" s="84">
-        <v>321</v>
+        <v>279</v>
+      </c>
+      <c r="D35" t="s" s="75">
+        <v>323</v>
+      </c>
+      <c r="E35" t="n" s="76">
+        <v>45.11425466614553</v>
       </c>
       <c r="G35" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H35" t="n" s="78">
-        <v>48.32602686486075</v>
-      </c>
-      <c r="I35" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>24.903070194239906</v>
+      </c>
+      <c r="H35" t="s" s="78">
+        <v>421</v>
       </c>
       <c r="K35" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L35" t="s" s="36">
-        <v>279</v>
-      </c>
-      <c r="M35" t="n" s="36">
-        <v>60.58933076252993</v>
-      </c>
-      <c r="AC35" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>71.80473372281939</v>
+      </c>
+      <c r="L35" t="n" s="36">
+        <v>14.473560420717712</v>
       </c>
     </row>
     <row r="36">
+      <c r="B36" t="n" s="34">
+        <v>66.5657324502926</v>
+      </c>
       <c r="C36" t="s" s="84">
-        <v>322</v>
+        <v>280</v>
+      </c>
+      <c r="D36" t="s" s="75">
+        <v>324</v>
+      </c>
+      <c r="E36" t="n" s="76">
+        <v>63.01362989762317</v>
       </c>
       <c r="G36" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H36" t="n" s="78">
-        <v>80.75637158136234</v>
-      </c>
-      <c r="I36" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>90.77807691653965</v>
+      </c>
+      <c r="H36" t="s" s="78">
+        <v>422</v>
       </c>
       <c r="K36" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L36" t="s" s="36">
-        <v>280</v>
-      </c>
-      <c r="M36" t="n" s="36">
-        <v>76.48796011887957</v>
-      </c>
-      <c r="AC36" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>18.814535659899988</v>
+      </c>
+      <c r="L36" t="n" s="36">
+        <v>23.93740018974394</v>
       </c>
     </row>
     <row r="37">
+      <c r="B37" t="n" s="34">
+        <v>50.43935055207817</v>
+      </c>
       <c r="C37" t="s" s="84">
-        <v>323</v>
+        <v>281</v>
+      </c>
+      <c r="D37" t="s" s="75">
+        <v>325</v>
+      </c>
+      <c r="E37" t="n" s="76">
+        <v>7.36794514075082</v>
       </c>
       <c r="G37" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H37" t="n" s="78">
-        <v>58.24346173231013</v>
-      </c>
-      <c r="I37" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>87.22054169361229</v>
+      </c>
+      <c r="H37" t="s" s="78">
+        <v>423</v>
       </c>
       <c r="K37" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L37" t="s" s="36">
-        <v>281</v>
-      </c>
-      <c r="M37" t="n" s="36">
-        <v>25.659377817007233</v>
-      </c>
-      <c r="AC37" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>13.65043497793591</v>
+      </c>
+      <c r="L37" t="n" s="36">
+        <v>70.30055458740291</v>
       </c>
     </row>
     <row r="38">
+      <c r="B38" t="n" s="34">
+        <v>36.50218865687576</v>
+      </c>
       <c r="C38" t="s" s="84">
-        <v>324</v>
+        <v>282</v>
+      </c>
+      <c r="D38" t="s" s="75">
+        <v>326</v>
+      </c>
+      <c r="E38" t="n" s="76">
+        <v>10.667315996393146</v>
       </c>
       <c r="G38" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H38" t="n" s="78">
-        <v>2.119842440341313</v>
-      </c>
-      <c r="I38" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>70.42394396398664</v>
+      </c>
+      <c r="H38" t="s" s="78">
+        <v>424</v>
       </c>
       <c r="K38" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L38" t="s" s="36">
-        <v>282</v>
-      </c>
-      <c r="M38" t="n" s="36">
-        <v>76.46809647382662</v>
-      </c>
-      <c r="AC38" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>96.94325755718651</v>
+      </c>
+      <c r="L38" t="n" s="36">
+        <v>57.76734018390067</v>
       </c>
     </row>
     <row r="39">
+      <c r="B39" t="n" s="34">
+        <v>27.74195821684462</v>
+      </c>
       <c r="C39" t="s" s="84">
-        <v>325</v>
+        <v>283</v>
+      </c>
+      <c r="D39" t="s" s="75">
+        <v>327</v>
+      </c>
+      <c r="E39" t="n" s="76">
+        <v>78.54976679768471</v>
       </c>
       <c r="G39" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H39" t="n" s="78">
-        <v>78.98802124593439</v>
-      </c>
-      <c r="I39" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>57.07048771867333</v>
+      </c>
+      <c r="H39" t="s" s="78">
+        <v>425</v>
       </c>
       <c r="K39" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L39" t="s" s="36">
-        <v>283</v>
-      </c>
-      <c r="M39" t="n" s="36">
-        <v>67.14418782489713</v>
-      </c>
-      <c r="AC39" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>66.25276348719044</v>
+      </c>
+      <c r="L39" t="n" s="36">
+        <v>9.849289813513117</v>
       </c>
     </row>
     <row r="40">
+      <c r="B40" t="n" s="34">
+        <v>7.80798327562342</v>
+      </c>
       <c r="C40" t="s" s="84">
-        <v>326</v>
+        <v>284</v>
+      </c>
+      <c r="D40" t="s" s="75">
+        <v>328</v>
+      </c>
+      <c r="E40" t="n" s="76">
+        <v>70.99842933579744</v>
       </c>
       <c r="G40" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H40" t="n" s="78">
-        <v>43.76077346504024</v>
-      </c>
-      <c r="I40" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>12.462038972494016</v>
+      </c>
+      <c r="H40" t="s" s="78">
+        <v>426</v>
       </c>
       <c r="K40" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L40" t="s" s="36">
-        <v>284</v>
-      </c>
-      <c r="M40" t="n" s="36">
-        <v>86.92818153163817</v>
-      </c>
-      <c r="AC40" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>63.10901595861391</v>
+      </c>
+      <c r="L40" t="n" s="36">
+        <v>58.81553378814487</v>
       </c>
     </row>
     <row r="41">
+      <c r="B41" t="n" s="34">
+        <v>27.994523943074125</v>
+      </c>
       <c r="C41" t="s" s="84">
-        <v>327</v>
+        <v>285</v>
+      </c>
+      <c r="D41" t="s" s="75">
+        <v>329</v>
+      </c>
+      <c r="E41" t="n" s="76">
+        <v>39.40155636202564</v>
       </c>
       <c r="G41" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H41" t="n" s="78">
-        <v>7.131429490982932</v>
-      </c>
-      <c r="I41" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>46.97953161824798</v>
+      </c>
+      <c r="H41" t="s" s="78">
+        <v>427</v>
       </c>
       <c r="K41" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L41" t="s" s="36">
-        <v>285</v>
-      </c>
-      <c r="M41" t="n" s="36">
-        <v>13.206075878385315</v>
-      </c>
-      <c r="AC41" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>70.96231539817384</v>
+      </c>
+      <c r="L41" t="n" s="36">
+        <v>86.29674311196493</v>
       </c>
     </row>
     <row r="42">
+      <c r="B42" t="n" s="34">
+        <v>77.28851091183984</v>
+      </c>
       <c r="C42" t="s" s="84">
-        <v>328</v>
+        <v>286</v>
+      </c>
+      <c r="D42" t="s" s="75">
+        <v>330</v>
+      </c>
+      <c r="E42" t="n" s="76">
+        <v>16.377235051078497</v>
       </c>
       <c r="G42" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H42" t="n" s="78">
-        <v>56.704724685840866</v>
-      </c>
-      <c r="I42" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>25.579089601483474</v>
+      </c>
+      <c r="H42" t="s" s="78">
+        <v>428</v>
       </c>
       <c r="K42" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L42" t="s" s="36">
-        <v>286</v>
-      </c>
-      <c r="M42" t="n" s="36">
-        <v>13.629166355531064</v>
-      </c>
-      <c r="AC42" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>20.54667601741359</v>
+      </c>
+      <c r="L42" t="n" s="36">
+        <v>80.52403395183907</v>
       </c>
     </row>
     <row r="43">
+      <c r="B43" t="n" s="34">
+        <v>37.88923092413988</v>
+      </c>
       <c r="C43" t="s" s="84">
-        <v>329</v>
+        <v>287</v>
+      </c>
+      <c r="D43" t="s" s="75">
+        <v>331</v>
+      </c>
+      <c r="E43" t="n" s="76">
+        <v>16.975362355107716</v>
       </c>
       <c r="G43" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H43" t="n" s="78">
-        <v>77.8216666891398</v>
+        <v>56.279882537708104</v>
+      </c>
+      <c r="H43" t="s" s="78">
+        <v>429</v>
       </c>
       <c r="K43" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L43" t="s" s="36">
-        <v>287</v>
-      </c>
-      <c r="M43" t="n" s="36">
-        <v>96.17828162696101</v>
-      </c>
-      <c r="AC43" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>16.154349081587462</v>
+      </c>
+      <c r="L43" t="n" s="36">
+        <v>95.74885428401576</v>
       </c>
     </row>
     <row r="44">
+      <c r="B44" t="n" s="34">
+        <v>82.73853722338134</v>
+      </c>
       <c r="C44" t="s" s="84">
-        <v>330</v>
+        <v>288</v>
+      </c>
+      <c r="D44" t="s" s="75">
+        <v>332</v>
+      </c>
+      <c r="E44" t="n" s="76">
+        <v>53.399991083918586</v>
       </c>
       <c r="G44" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H44" t="n" s="78">
-        <v>34.142735305213876</v>
+        <v>55.38305400931507</v>
+      </c>
+      <c r="H44" t="s" s="78">
+        <v>430</v>
       </c>
       <c r="K44" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L44" t="s" s="36">
-        <v>288</v>
-      </c>
-      <c r="M44" t="n" s="36">
-        <v>65.98478774317803</v>
+        <v>65.79889981095667</v>
+      </c>
+      <c r="L44" t="n" s="36">
+        <v>56.193461099447084</v>
       </c>
     </row>
     <row r="45">
+      <c r="B45" t="n" s="34">
+        <v>14.700110600705319</v>
+      </c>
       <c r="C45" t="s" s="84">
-        <v>331</v>
+        <v>289</v>
+      </c>
+      <c r="D45" t="s" s="75">
+        <v>333</v>
+      </c>
+      <c r="E45" t="n" s="76">
+        <v>33.65180440191422</v>
       </c>
       <c r="G45" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H45" t="n" s="78">
-        <v>69.48882808292946</v>
+        <v>76.97495908839261</v>
+      </c>
+      <c r="H45" t="s" s="78">
+        <v>431</v>
       </c>
       <c r="K45" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L45" t="s" s="36">
-        <v>289</v>
-      </c>
-      <c r="M45" t="n" s="36">
-        <v>29.714827498801842</v>
+        <v>21.733073816946767</v>
+      </c>
+      <c r="L45" t="n" s="36">
+        <v>87.68509826578325</v>
       </c>
     </row>
     <row r="46">
+      <c r="B46" t="n" s="34">
+        <v>68.28511916668467</v>
+      </c>
       <c r="C46" t="s" s="84">
-        <v>332</v>
+        <v>290</v>
+      </c>
+      <c r="D46" t="s" s="75">
+        <v>334</v>
+      </c>
+      <c r="E46" t="n" s="76">
+        <v>52.72082365337718</v>
       </c>
       <c r="G46" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H46" t="n" s="78">
-        <v>1.6168210289827067</v>
+        <v>7.499749195633509</v>
+      </c>
+      <c r="H46" t="s" s="78">
+        <v>432</v>
       </c>
       <c r="K46" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L46" t="s" s="36">
-        <v>290</v>
-      </c>
-      <c r="M46" t="n" s="36">
-        <v>11.990426865400728</v>
+        <v>69.80741692879886</v>
+      </c>
+      <c r="L46" t="n" s="36">
+        <v>35.875873709528605</v>
       </c>
     </row>
     <row r="47">
+      <c r="B47" t="n" s="34">
+        <v>83.5722054551965</v>
+      </c>
       <c r="C47" t="s" s="84">
-        <v>333</v>
+        <v>291</v>
+      </c>
+      <c r="D47" t="s" s="75">
+        <v>335</v>
+      </c>
+      <c r="E47" t="n" s="76">
+        <v>78.4055718104755</v>
       </c>
       <c r="G47" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H47" t="n" s="78">
-        <v>95.6894742986167</v>
+        <v>23.412918300105723</v>
+      </c>
+      <c r="H47" t="s" s="78">
+        <v>433</v>
       </c>
       <c r="K47" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="L47" t="s" s="36">
-        <v>291</v>
-      </c>
-      <c r="M47" t="n" s="36">
-        <v>5.6726678908190165</v>
+        <v>47.936096681401864</v>
+      </c>
+      <c r="L47" t="n" s="36">
+        <v>10.075156740764335</v>
       </c>
     </row>
     <row r="48">
+      <c r="B48" t="n" s="34">
+        <v>91.82695767792575</v>
+      </c>
       <c r="C48" t="s" s="84">
-        <v>334</v>
+        <v>292</v>
+      </c>
+      <c r="D48" t="s" s="75">
+        <v>336</v>
+      </c>
+      <c r="E48" t="n" s="76">
+        <v>51.8790420159433</v>
       </c>
       <c r="G48" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H48" t="n" s="78">
-        <v>65.55409896000722</v>
+        <v>28.12089397099321</v>
+      </c>
+      <c r="H48" t="s" s="78">
+        <v>434</v>
       </c>
       <c r="K48" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M48" t="n" s="36">
-        <v>79.13275893017475</v>
+        <v>3.3043797808555153</v>
+      </c>
+      <c r="L48" t="n" s="36">
+        <v>8.870822953322755</v>
       </c>
     </row>
     <row r="49">
+      <c r="B49" t="n" s="34">
+        <v>6.191694186936314</v>
+      </c>
       <c r="C49" t="s" s="84">
-        <v>335</v>
+        <v>293</v>
+      </c>
+      <c r="D49" t="s" s="75">
+        <v>337</v>
+      </c>
+      <c r="E49" t="n" s="76">
+        <v>70.31911390589396</v>
       </c>
       <c r="G49" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H49" t="n" s="78">
-        <v>5.370278311348575</v>
+        <v>54.32853188943431</v>
+      </c>
+      <c r="H49" t="s" s="78">
+        <v>435</v>
       </c>
       <c r="K49" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M49" t="n" s="36">
-        <v>64.26622119243567</v>
+        <v>23.29285723326725</v>
+      </c>
+      <c r="L49" t="n" s="36">
+        <v>46.31097997097046</v>
       </c>
     </row>
     <row r="50">
-      <c r="C50" t="s" s="84">
-        <v>336</v>
+      <c r="B50" t="n" s="34">
+        <v>22.145418646418445</v>
+      </c>
+      <c r="D50" t="s" s="75">
+        <v>338</v>
+      </c>
+      <c r="E50" t="n" s="76">
+        <v>33.930311886721064</v>
       </c>
       <c r="G50" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H50" t="n" s="78">
-        <v>83.70735384976437</v>
+        <v>5.558523516960134</v>
+      </c>
+      <c r="H50" t="s" s="78">
+        <v>436</v>
       </c>
       <c r="K50" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M50" t="n" s="36">
-        <v>35.5478955659087</v>
+        <v>41.89815993247913</v>
+      </c>
+      <c r="L50" t="n" s="36">
+        <v>48.54639393334635</v>
       </c>
     </row>
     <row r="51">
-      <c r="C51" t="s" s="84">
-        <v>337</v>
+      <c r="B51" t="n" s="34">
+        <v>58.77571617684947</v>
+      </c>
+      <c r="D51" t="s" s="75">
+        <v>339</v>
+      </c>
+      <c r="E51" t="n" s="76">
+        <v>48.74109808284619</v>
       </c>
       <c r="G51" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H51" t="n" s="78">
-        <v>23.193019274979232</v>
+        <v>11.270757666532782</v>
+      </c>
+      <c r="H51" t="s" s="78">
+        <v>437</v>
       </c>
       <c r="K51" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M51" t="n" s="36">
-        <v>10.75517840786543</v>
+        <v>67.57568386940976</v>
+      </c>
+      <c r="L51" t="n" s="36">
+        <v>57.61942645284586</v>
       </c>
     </row>
     <row r="52">
-      <c r="C52" t="s" s="84">
-        <v>338</v>
+      <c r="B52" t="n" s="34">
+        <v>82.36006193279694</v>
+      </c>
+      <c r="D52" t="s" s="75">
+        <v>340</v>
+      </c>
+      <c r="E52" t="n" s="76">
+        <v>98.75906975618761</v>
       </c>
       <c r="G52" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H52" t="n" s="78">
-        <v>33.38937835605198</v>
+        <v>49.06439969866475</v>
+      </c>
+      <c r="H52" t="s" s="78">
+        <v>438</v>
       </c>
       <c r="K52" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M52" t="n" s="36">
-        <v>41.73541605180896</v>
+        <v>10.949164632960883</v>
+      </c>
+      <c r="L52" t="n" s="36">
+        <v>47.304858367180145</v>
       </c>
     </row>
     <row r="53">
+      <c r="B53" t="n" s="34">
+        <v>2.615162563860529</v>
+      </c>
+      <c r="D53" t="s" s="75">
+        <v>341</v>
+      </c>
+      <c r="E53" t="n" s="76">
+        <v>18.331193357968502</v>
+      </c>
       <c r="G53" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H53" t="n" s="78">
-        <v>19.63515192890466</v>
+        <v>52.603432875339905</v>
+      </c>
+      <c r="H53" t="s" s="78">
+        <v>439</v>
       </c>
       <c r="K53" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M53" t="n" s="36">
-        <v>98.02062324828292</v>
+        <v>14.571236498273377</v>
+      </c>
+      <c r="L53" t="n" s="36">
+        <v>20.24060610338969</v>
       </c>
     </row>
     <row r="54">
+      <c r="B54" t="n" s="34">
+        <v>6.433120696944727</v>
+      </c>
+      <c r="D54" t="s" s="75">
+        <v>342</v>
+      </c>
+      <c r="E54" t="n" s="76">
+        <v>40.837157807814194</v>
+      </c>
       <c r="G54" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H54" t="n" s="78">
-        <v>16.016957309637426</v>
+        <v>29.38080306631079</v>
+      </c>
+      <c r="H54" t="s" s="78">
+        <v>440</v>
       </c>
       <c r="K54" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M54" t="n" s="36">
-        <v>3.9961563241472597</v>
+        <v>86.09340881095466</v>
+      </c>
+      <c r="L54" t="n" s="36">
+        <v>36.51489727293308</v>
       </c>
     </row>
     <row r="55">
+      <c r="D55" t="s" s="75">
+        <v>343</v>
+      </c>
+      <c r="E55" t="n" s="76">
+        <v>82.6561149304178</v>
+      </c>
       <c r="G55" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H55" t="n" s="78">
-        <v>5.680095801059782</v>
+        <v>35.997347246360626</v>
+      </c>
+      <c r="H55" t="s" s="78">
+        <v>441</v>
       </c>
       <c r="K55" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M55" t="n" s="36">
-        <v>87.2620602461316</v>
+        <v>45.497104710298416</v>
+      </c>
+      <c r="L55" t="n" s="36">
+        <v>7.878731334713329</v>
       </c>
     </row>
     <row r="56">
+      <c r="D56" t="s" s="75">
+        <v>344</v>
+      </c>
+      <c r="E56" t="n" s="76">
+        <v>0.4349992708124639</v>
+      </c>
       <c r="G56" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H56" t="n" s="78">
-        <v>27.630677583283124</v>
+        <v>58.204907406749726</v>
+      </c>
+      <c r="H56" t="s" s="78">
+        <v>442</v>
       </c>
       <c r="K56" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M56" t="n" s="36">
-        <v>79.50885584634578</v>
+        <v>47.50462149942558</v>
+      </c>
+      <c r="L56" t="n" s="36">
+        <v>42.049366056119595</v>
       </c>
     </row>
     <row r="57">
+      <c r="D57" t="s" s="75">
+        <v>345</v>
+      </c>
       <c r="G57" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H57" t="n" s="78">
-        <v>62.41773949249285</v>
+        <v>90.03376207320399</v>
+      </c>
+      <c r="H57" t="s" s="78">
+        <v>443</v>
       </c>
       <c r="K57" t="n" s="36">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="M57" t="n" s="36">
-        <v>60.681690927868544</v>
+        <v>94.9599217003524</v>
+      </c>
+      <c r="L57" t="n" s="36">
+        <v>22.322188633485183</v>
       </c>
     </row>
     <row r="58">
+      <c r="D58" t="s" s="75">
+        <v>346</v>
+      </c>
       <c r="G58" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H58" t="n" s="78">
-        <v>49.51385269929354</v>
+        <v>9.03928160798374</v>
+      </c>
+      <c r="H58" t="s" s="78">
+        <v>444</v>
       </c>
       <c r="K58" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>91.66228476470829</v>
+      </c>
+      <c r="L58" t="n" s="36">
+        <v>45.17199030001525</v>
       </c>
     </row>
     <row r="59">
+      <c r="D59" t="s" s="75">
+        <v>347</v>
+      </c>
       <c r="G59" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H59" t="n" s="78">
-        <v>94.22992071536605</v>
+        <v>14.18485743023663</v>
+      </c>
+      <c r="H59" t="s" s="78">
+        <v>445</v>
       </c>
       <c r="K59" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>19.626245113055507</v>
+      </c>
+      <c r="L59" t="n" s="36">
+        <v>88.31656859318792</v>
       </c>
     </row>
     <row r="60">
+      <c r="D60" t="s" s="75">
+        <v>348</v>
+      </c>
       <c r="G60" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H60" t="n" s="78">
-        <v>27.145658295040054</v>
+        <v>71.89470045283062</v>
+      </c>
+      <c r="H60" t="s" s="78">
+        <v>446</v>
       </c>
       <c r="K60" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>57.04845257525283</v>
+      </c>
+      <c r="L60" t="n" s="36">
+        <v>61.943253487277275</v>
       </c>
     </row>
     <row r="61">
+      <c r="D61" t="s" s="75">
+        <v>349</v>
+      </c>
       <c r="G61" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H61" t="n" s="78">
-        <v>1.941715285786627</v>
+        <v>79.56070066211612</v>
+      </c>
+      <c r="H61" t="s" s="78">
+        <v>447</v>
       </c>
       <c r="K61" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>46.4472028951968</v>
+      </c>
+      <c r="L61" t="n" s="36">
+        <v>61.449950648303464</v>
       </c>
     </row>
     <row r="62">
+      <c r="D62" t="s" s="75">
+        <v>350</v>
+      </c>
       <c r="G62" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H62" t="n" s="78">
-        <v>42.399866755343375</v>
+        <v>10.199873802086346</v>
+      </c>
+      <c r="H62" t="s" s="78">
+        <v>448</v>
       </c>
       <c r="K62" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>94.92799336586606</v>
+      </c>
+      <c r="L62" t="n" s="36">
+        <v>34.662784029253835</v>
       </c>
     </row>
     <row r="63">
+      <c r="D63" t="s" s="75">
+        <v>351</v>
+      </c>
       <c r="G63" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H63" t="n" s="78">
-        <v>14.943632689273423</v>
+        <v>45.51298152250003</v>
+      </c>
+      <c r="H63" t="s" s="78">
+        <v>449</v>
       </c>
       <c r="K63" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>77.59617138196438</v>
+      </c>
+      <c r="L63" t="n" s="36">
+        <v>22.727737475160538</v>
       </c>
     </row>
     <row r="64">
+      <c r="D64" t="s" s="75">
+        <v>352</v>
+      </c>
       <c r="G64" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H64" t="n" s="78">
-        <v>77.61443670196935</v>
+        <v>85.30988224739866</v>
+      </c>
+      <c r="H64" t="s" s="78">
+        <v>450</v>
       </c>
       <c r="K64" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>64.83531403790498</v>
+      </c>
+      <c r="L64" t="n" s="36">
+        <v>35.29298373557616</v>
       </c>
     </row>
     <row r="65">
-      <c r="G65" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H65" t="n" s="78">
-        <v>68.4612609356489</v>
+      <c r="D65" t="s" s="75">
+        <v>353</v>
+      </c>
+      <c r="H65" t="s" s="78">
+        <v>451</v>
       </c>
       <c r="K65" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>97.56235503925726</v>
+      </c>
+      <c r="L65" t="n" s="36">
+        <v>62.491096523795854</v>
       </c>
     </row>
     <row r="66">
-      <c r="G66" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H66" t="n" s="78">
-        <v>81.94340062397507</v>
+      <c r="D66" t="s" s="75">
+        <v>354</v>
+      </c>
+      <c r="H66" t="s" s="78">
+        <v>452</v>
       </c>
       <c r="K66" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>9.818270075667247</v>
+      </c>
+      <c r="L66" t="n" s="36">
+        <v>4.038954645154014</v>
       </c>
     </row>
     <row r="67">
-      <c r="G67" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H67" t="n" s="78">
-        <v>22.558764794129914</v>
+      <c r="D67" t="s" s="75">
+        <v>355</v>
+      </c>
+      <c r="H67" t="s" s="78">
+        <v>453</v>
       </c>
       <c r="K67" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>42.47045177802051</v>
+      </c>
+      <c r="L67" t="n" s="36">
+        <v>65.24771803581723</v>
       </c>
     </row>
     <row r="68">
-      <c r="G68" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H68" t="n" s="78">
-        <v>92.85898764876973</v>
+      <c r="D68" t="s" s="75">
+        <v>356</v>
+      </c>
+      <c r="H68" t="s" s="78">
+        <v>454</v>
       </c>
       <c r="K68" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>48.66191240119836</v>
+      </c>
+      <c r="L68" t="n" s="36">
+        <v>3.5782817300503478</v>
       </c>
     </row>
     <row r="69">
-      <c r="G69" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H69" t="n" s="78">
-        <v>65.86508289305827</v>
+      <c r="D69" t="s" s="75">
+        <v>357</v>
+      </c>
+      <c r="H69" t="s" s="78">
+        <v>455</v>
       </c>
       <c r="K69" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>80.10957275394979</v>
+      </c>
+      <c r="L69" t="n" s="36">
+        <v>60.77725330841146</v>
       </c>
     </row>
     <row r="70">
-      <c r="G70" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H70" t="n" s="78">
-        <v>27.958622242878516</v>
+      <c r="D70" t="s" s="75">
+        <v>358</v>
+      </c>
+      <c r="H70" t="s" s="78">
+        <v>456</v>
       </c>
       <c r="K70" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>42.578857728930544</v>
+      </c>
+      <c r="L70" t="n" s="36">
+        <v>29.68856051550822</v>
       </c>
     </row>
     <row r="71">
-      <c r="G71" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H71" t="n" s="78">
-        <v>41.22277702316532</v>
+      <c r="D71" t="s" s="75">
+        <v>359</v>
+      </c>
+      <c r="H71" t="s" s="78">
+        <v>457</v>
       </c>
       <c r="K71" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>52.856650719842015</v>
+      </c>
+      <c r="L71" t="n" s="36">
+        <v>84.5505726461169</v>
       </c>
     </row>
     <row r="72">
-      <c r="G72" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H72" t="n" s="78">
-        <v>35.071257680505596</v>
+      <c r="D72" t="s" s="75">
+        <v>360</v>
+      </c>
+      <c r="H72" t="s" s="78">
+        <v>458</v>
       </c>
       <c r="K72" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>60.11927925863395</v>
+      </c>
+      <c r="L72" t="n" s="36">
+        <v>27.62072091608433</v>
       </c>
     </row>
     <row r="73">
-      <c r="G73" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H73" t="n" s="78">
-        <v>48.3585120752867</v>
+      <c r="D73" t="s" s="75">
+        <v>361</v>
+      </c>
+      <c r="H73" t="s" s="78">
+        <v>459</v>
       </c>
       <c r="K73" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>35.23749556029359</v>
+      </c>
+      <c r="L73" t="n" s="36">
+        <v>10.128265074824583</v>
       </c>
     </row>
     <row r="74">
-      <c r="G74" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H74" t="n" s="78">
-        <v>89.3352658495125</v>
+      <c r="D74" t="s" s="75">
+        <v>362</v>
+      </c>
+      <c r="H74" t="s" s="78">
+        <v>460</v>
       </c>
       <c r="K74" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>85.79459462053394</v>
+      </c>
+      <c r="L74" t="n" s="36">
+        <v>67.48512304414672</v>
       </c>
     </row>
     <row r="75">
-      <c r="G75" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H75" t="n" s="78">
-        <v>85.20216026339004</v>
+      <c r="D75" t="s" s="75">
+        <v>363</v>
+      </c>
+      <c r="H75" t="s" s="78">
+        <v>461</v>
       </c>
       <c r="K75" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>97.91115236109266</v>
+      </c>
+      <c r="L75" t="n" s="36">
+        <v>59.90835917644627</v>
       </c>
     </row>
     <row r="76">
-      <c r="G76" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H76" t="n" s="78">
-        <v>23.283874750492096</v>
+      <c r="D76" t="s" s="75">
+        <v>364</v>
+      </c>
+      <c r="H76" t="s" s="78">
+        <v>462</v>
       </c>
       <c r="K76" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>31.16009209432711</v>
+      </c>
+      <c r="L76" t="n" s="36">
+        <v>4.689904879967932</v>
       </c>
     </row>
     <row r="77">
-      <c r="G77" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H77" t="n" s="78">
-        <v>63.64273829054184</v>
+      <c r="D77" t="s" s="75">
+        <v>365</v>
+      </c>
+      <c r="H77" t="s" s="78">
+        <v>463</v>
       </c>
       <c r="K77" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>84.08172561431286</v>
+      </c>
+      <c r="L77" t="n" s="36">
+        <v>39.567630256259754</v>
       </c>
     </row>
     <row r="78">
-      <c r="G78" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H78" t="n" s="78">
-        <v>15.4336698390385</v>
+      <c r="D78" t="s" s="75">
+        <v>366</v>
+      </c>
+      <c r="H78" t="s" s="78">
+        <v>464</v>
       </c>
       <c r="K78" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>99.46049445518624</v>
+      </c>
+      <c r="L78" t="n" s="36">
+        <v>18.195169597056093</v>
       </c>
     </row>
     <row r="79">
-      <c r="G79" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H79" t="n" s="78">
-        <v>95.3699541259484</v>
+      <c r="D79" t="s" s="75">
+        <v>367</v>
+      </c>
+      <c r="H79" t="s" s="78">
+        <v>465</v>
       </c>
       <c r="K79" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>40.490267457555106</v>
+      </c>
+      <c r="L79" t="n" s="36">
+        <v>61.03895950240575</v>
       </c>
     </row>
     <row r="80">
-      <c r="G80" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H80" t="n" s="78">
-        <v>91.39996412486914</v>
+      <c r="D80" t="s" s="75">
+        <v>368</v>
+      </c>
+      <c r="H80" t="s" s="78">
+        <v>466</v>
       </c>
       <c r="K80" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>90.56903183711823</v>
       </c>
     </row>
     <row r="81">
-      <c r="G81" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H81" t="n" s="78">
-        <v>71.13913424902708</v>
+      <c r="D81" t="s" s="75">
+        <v>369</v>
+      </c>
+      <c r="H81" t="s" s="78">
+        <v>467</v>
       </c>
       <c r="K81" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>90.03418702274189</v>
       </c>
     </row>
     <row r="82">
-      <c r="G82" t="n" s="77">
-        <v>44964.71703053241</v>
-      </c>
-      <c r="H82" t="n" s="78">
-        <v>82.69473301282079</v>
+      <c r="D82" t="s" s="75">
+        <v>370</v>
+      </c>
+      <c r="H82" t="s" s="78">
+        <v>468</v>
       </c>
       <c r="K82" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>77.56774449076994</v>
       </c>
     </row>
     <row r="83">
-      <c r="G83" t="n" s="77">
-        <v>44964.71703053241</v>
+      <c r="D83" t="s" s="75">
+        <v>371</v>
+      </c>
+      <c r="H83" t="s" s="78">
+        <v>469</v>
       </c>
       <c r="K83" t="n" s="36">
-        <v>44964.71703053241</v>
+        <v>37.58156595333473</v>
       </c>
     </row>
     <row r="84">
-      <c r="G84" t="n" s="77">
-        <v>44964.71703053241</v>
+      <c r="D84" t="s" s="75">
+        <v>372</v>
+      </c>
+      <c r="H84" t="s" s="78">
+        <v>470</v>
+      </c>
+      <c r="K84" t="n" s="36">
+        <v>32.209370784907485</v>
       </c>
     </row>
     <row r="85">
-      <c r="G85" t="n" s="77">
-        <v>44964.71703053241</v>
+      <c r="D85" t="s" s="75">
+        <v>373</v>
+      </c>
+      <c r="H85" t="s" s="78">
+        <v>471</v>
+      </c>
+      <c r="K85" t="n" s="36">
+        <v>4.634560143201605</v>
       </c>
     </row>
     <row r="86">
-      <c r="G86" t="n" s="77">
-        <v>44964.71703053241</v>
+      <c r="D86" t="s" s="75">
+        <v>374</v>
+      </c>
+      <c r="H86" t="s" s="78">
+        <v>472</v>
+      </c>
+      <c r="K86" t="n" s="36">
+        <v>67.51724847944512</v>
       </c>
     </row>
     <row r="87">
-      <c r="G87" t="n" s="77">
-        <v>44964.71703053241</v>
+      <c r="D87" t="s" s="75">
+        <v>375</v>
+      </c>
+      <c r="H87" t="s" s="78">
+        <v>473</v>
+      </c>
+      <c r="K87" t="n" s="36">
+        <v>46.15323868738964</v>
       </c>
     </row>
     <row r="88">
-      <c r="G88" t="n" s="77">
-        <v>44964.71703053241</v>
+      <c r="D88" t="s" s="75">
+        <v>376</v>
+      </c>
+      <c r="H88" t="s" s="78">
+        <v>474</v>
+      </c>
+      <c r="K88" t="n" s="36">
+        <v>22.329087127711134</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="D89" t="s" s="75">
+        <v>377</v>
+      </c>
+      <c r="H89" t="s" s="78">
+        <v>475</v>
+      </c>
+      <c r="K89" t="n" s="36">
+        <v>7.145426339339755</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="D90" t="s" s="75">
+        <v>378</v>
+      </c>
+      <c r="H90" t="s" s="78">
+        <v>476</v>
+      </c>
+      <c r="K90" t="n" s="36">
+        <v>56.64599681395865</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="D91" t="s" s="75">
+        <v>379</v>
+      </c>
+      <c r="H91" t="s" s="78">
+        <v>477</v>
+      </c>
+      <c r="K91" t="n" s="36">
+        <v>84.68822472423228</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="D92" t="s" s="75">
+        <v>380</v>
+      </c>
+      <c r="H92" t="s" s="78">
+        <v>478</v>
+      </c>
+      <c r="K92" t="n" s="36">
+        <v>6.745031047033678</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="D93" t="s" s="75">
+        <v>381</v>
+      </c>
+      <c r="H93" t="s" s="78">
+        <v>479</v>
+      </c>
+      <c r="K93" t="n" s="36">
+        <v>19.064190390376133</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="D94" t="s" s="75">
+        <v>382</v>
+      </c>
+      <c r="H94" t="s" s="78">
+        <v>480</v>
+      </c>
+      <c r="K94" t="n" s="36">
+        <v>65.24920381280798</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="D95" t="s" s="75">
+        <v>383</v>
+      </c>
+      <c r="K95" t="n" s="36">
+        <v>5.923714916011614</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="D96" t="s" s="75">
+        <v>384</v>
+      </c>
+      <c r="K96" t="n" s="36">
+        <v>80.38372871301422</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="D97" t="s" s="75">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="D98" t="s" s="75">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="D99" t="s" s="75">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="D100" t="s" s="75">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="D101" t="s" s="75">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="D102" t="s" s="75">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="D103" t="s" s="75">
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -9238,7 +9979,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A75BBA-F9EE-440E-92CB-DE0F3D7743BE}">
-  <dimension ref="A2:G54"/>
+  <dimension ref="A2:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
@@ -9248,45 +9989,35 @@
   <sheetData>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>61.62893314646563</v>
+        <v>5.960507509959811</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>6.442140441255228</v>
+        <v>57.30158822341417</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="A4" t="n" s="0">
-        <v>89.34026198256646</v>
+        <v>93.80816071451198</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>4.3248472661971675</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>6.677976306260372</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>3.660870520851189</v>
-      </c>
+        <v>0.15321380318431999</v>
+      </c>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
     </row>
     <row r="5" spans="5:7">
       <c r="A5" t="n" s="0">
-        <v>40.3110546911858</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>5.7549165338685455</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>4.60084960817957</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>6.311987283978248</v>
-      </c>
+        <v>5.375094309750061</v>
+      </c>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
     </row>
     <row r="6" spans="5:7">
       <c r="A6" t="n" s="0">
-        <v>23.274365863470294</v>
+        <v>33.09096960503961</v>
       </c>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
@@ -9294,242 +10025,77 @@
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>25.857171497100428</v>
+        <v>75.68130333940954</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>53.70808245406824</v>
+        <v>22.840212733242858</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n" s="0">
-        <v>16.394957547261903</v>
+        <v>89.310875189177</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n" s="0">
-        <v>16.419157395488625</v>
+        <v>46.6184406082191</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n" s="0">
-        <v>2.8198863260423312</v>
+        <v>94.0974083352657</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n" s="0">
-        <v>0.04028071807258282</v>
+        <v>47.78438629125702</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n" s="0">
-        <v>70.52690353100985</v>
+        <v>25.909658169082185</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n" s="0">
-        <v>65.5756296351826</v>
+        <v>1.9880874510478042</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n" s="0">
-        <v>53.787888572976286</v>
+        <v>22.76331011679027</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n" s="0">
-        <v>53.548219744188465</v>
+        <v>63.11403269229976</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n" s="0">
-        <v>60.54880251872925</v>
+        <v>62.365014457852155</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n" s="0">
-        <v>69.00802288462171</v>
+        <v>15.625865857852938</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n" s="0">
-        <v>80.62837019981735</v>
+        <v>94.10467752339153</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n" s="0">
-        <v>90.95149347542113</v>
+        <v>40.83004371157507</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n" s="0">
-        <v>84.62419185130649</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n" s="0">
-        <v>26.461358811895085</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n" s="0">
-        <v>86.74448442611282</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n" s="0">
-        <v>86.0130636748329</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n" s="0">
-        <v>51.1316750185583</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n" s="0">
-        <v>73.91475463351931</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n" s="0">
-        <v>13.43801851500136</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n" s="0">
-        <v>84.81767482755455</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n" s="0">
-        <v>14.42606666254813</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n" s="0">
-        <v>55.7822056786414</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n" s="0">
-        <v>73.73309799412269</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n" s="0">
-        <v>14.702896626123152</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n" s="0">
-        <v>94.75642639458445</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n" s="0">
-        <v>75.23769518437464</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n" s="0">
-        <v>87.54582141571913</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n" s="0">
-        <v>80.06841757659264</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n" s="0">
-        <v>28.852844403914634</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n" s="0">
-        <v>76.7204263476188</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n" s="0">
-        <v>76.8698530195615</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n" s="0">
-        <v>0.7308030372524477</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n" s="0">
-        <v>4.041436125528208</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n" s="0">
-        <v>31.17985628602532</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n" s="0">
-        <v>62.55817460309531</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n" s="0">
-        <v>4.057148107450592</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n" s="0">
-        <v>13.219745278209716</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n" s="0">
-        <v>14.24915341784957</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n" s="0">
-        <v>15.316366861390286</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n" s="0">
-        <v>90.80261100633969</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n" s="0">
-        <v>30.622329967533503</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n" s="0">
-        <v>90.28954835555756</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n" s="0">
-        <v>52.68292165253429</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n" s="0">
-        <v>56.39313669598893</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n" s="0">
-        <v>49.02901180497761</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n" s="0">
-        <v>41.12704661015193</v>
+        <v>49.51890522457061</v>
       </c>
     </row>
   </sheetData>
@@ -9547,22 +10113,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>339</v>
+        <v>481</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>346</v>
+        <v>488</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>356</v>
+        <v>498</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>366</v>
+        <v>508</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>376</v>
+        <v>518</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>386</v>
+        <v>528</v>
       </c>
       <c r="G1" t="n" s="0">
         <v>0.021</v>
@@ -9570,22 +10136,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>340</v>
+        <v>482</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>347</v>
+        <v>489</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>357</v>
+        <v>499</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>367</v>
+        <v>509</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>377</v>
+        <v>519</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>387</v>
+        <v>529</v>
       </c>
       <c r="G2" t="n" s="0">
         <v>100.3</v>
@@ -9593,22 +10159,22 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>341</v>
+        <v>483</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>348</v>
+        <v>490</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>358</v>
+        <v>500</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>368</v>
+        <v>510</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>378</v>
+        <v>520</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>388</v>
+        <v>530</v>
       </c>
       <c r="G3" t="n" s="0">
         <v>9.275</v>
@@ -9616,19 +10182,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>342</v>
+        <v>484</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>349</v>
+        <v>491</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>359</v>
+        <v>501</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>369</v>
+        <v>511</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>379</v>
+        <v>521</v>
       </c>
       <c r="G4" t="n" s="0">
         <v>100000.734</v>
@@ -9636,95 +10202,95 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>343</v>
+        <v>485</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>350</v>
+        <v>492</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>360</v>
+        <v>502</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>370</v>
+        <v>512</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>380</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>344</v>
+        <v>486</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>351</v>
+        <v>493</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>361</v>
+        <v>503</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>371</v>
+        <v>513</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>381</v>
+        <v>523</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>345</v>
+        <v>487</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>352</v>
+        <v>494</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>362</v>
+        <v>504</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>372</v>
+        <v>514</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>382</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="0">
-        <v>353</v>
+        <v>495</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>363</v>
+        <v>505</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>373</v>
+        <v>515</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>383</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s" s="0">
-        <v>354</v>
+        <v>496</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>364</v>
+        <v>506</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>374</v>
+        <v>516</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>384</v>
+        <v>526</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s" s="0">
-        <v>355</v>
+        <v>497</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>365</v>
+        <v>507</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>375</v>
+        <v>517</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>385</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>